<commit_message>
updated the Project plan docks
updated the documentation to reflect the project changes and our group's progress
</commit_message>
<xml_diff>
--- a/Project_Plan_Docs/CSC_289_Group_2_Project_Backlog.xlsx
+++ b/Project_Plan_Docs/CSC_289_Group_2_Project_Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programming Capstone Project\Inventory-Management-System\Project_Plan_Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\docto\Documents\Programming Capstone Project\Inventory-Management-System\Project_Plan_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B189B6A5-1756-4480-B076-4FF4642C5B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00768C8A-A384-40D4-A64D-040808753696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7E6936B-90AD-4E41-93D8-8E23721F7813}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7E6936B-90AD-4E41-93D8-8E23721F7813}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>TASK ID</t>
   </si>
@@ -118,13 +118,19 @@
     <t>Select the application Medium</t>
   </si>
   <si>
-    <t>Donovan Ester</t>
-  </si>
-  <si>
-    <t>Kameron Smith</t>
-  </si>
-  <si>
     <t>Set Up environment</t>
+  </si>
+  <si>
+    <t>Select the language to be utilized</t>
+  </si>
+  <si>
+    <t>Walker (Mentor)</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Kameron Smith and  Walker (Mentor)</t>
   </si>
 </sst>
 </file>
@@ -768,7 +774,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +859,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E3" s="8">
         <v>45691</v>
@@ -865,7 +871,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>11</v>
@@ -883,22 +889,22 @@
         <v>1.2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="8">
         <v>45692</v>
       </c>
       <c r="F4" s="8">
-        <v>45692</v>
+        <v>45704</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>11</v>
@@ -919,13 +925,27 @@
       <c r="B5" s="7">
         <v>1.3</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="8">
+        <v>45695</v>
+      </c>
+      <c r="F5" s="8">
+        <v>45695</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="9" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
got micro-ui to run
was able to get a demo project up and running utilizing the micro-ui package.
</commit_message>
<xml_diff>
--- a/Project_Plan_Docs/CSC_289_Group_2_Project_Backlog.xlsx
+++ b/Project_Plan_Docs/CSC_289_Group_2_Project_Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\docto\Documents\Programming Capstone Project\Inventory-Management-System\Project_Plan_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE98128F-6210-4717-A8AA-E9D72CBA445C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BF8CBE-A45B-4293-9C4A-40C806351D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{C7E6936B-90AD-4E41-93D8-8E23721F7813}"/>
+    <workbookView xWindow="2730" yWindow="4140" windowWidth="21600" windowHeight="11835" xr2:uid="{C7E6936B-90AD-4E41-93D8-8E23721F7813}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>TASK ID</t>
   </si>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7569EC-639A-4E4B-A266-3414136787BC}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,8 +1070,12 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1089,8 +1093,12 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -1108,8 +1116,12 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1123,7 +1135,9 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="I13" s="7"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>

</xml_diff>

<commit_message>
got a larger ui-demo to work
</commit_message>
<xml_diff>
--- a/Project_Plan_Docs/CSC_289_Group_2_Project_Backlog.xlsx
+++ b/Project_Plan_Docs/CSC_289_Group_2_Project_Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\docto\Documents\Programming Capstone Project\Inventory-Management-System\Project_Plan_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BF8CBE-A45B-4293-9C4A-40C806351D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4094F9B7-E452-4324-BAF3-31F5204D18E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="4140" windowWidth="21600" windowHeight="11835" xr2:uid="{C7E6936B-90AD-4E41-93D8-8E23721F7813}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7E6936B-90AD-4E41-93D8-8E23721F7813}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>TASK ID</t>
   </si>
@@ -148,10 +148,25 @@
     <t>Donovan Ester, Timothy Barton</t>
   </si>
   <si>
-    <t>Unit testing</t>
-  </si>
-  <si>
     <t>CJ Coronado, Kameron Smith</t>
+  </si>
+  <si>
+    <t>Binary Database integration with class sytem</t>
+  </si>
+  <si>
+    <t>Robert Snyder, CJ Coronado, Ethan Bevier</t>
+  </si>
+  <si>
+    <t>refine Micro UI</t>
+  </si>
+  <si>
+    <t>Donovan Ester, Kameron Smith, Peter Jiayu Zhang</t>
+  </si>
+  <si>
+    <t>Floater (you'll help where it's needed)</t>
+  </si>
+  <si>
+    <t>Timothy Barton</t>
   </si>
 </sst>
 </file>
@@ -795,7 +810,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,10 +1080,15 @@
         <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10:E12" si="0">E9</f>
+        <v>45705</v>
+      </c>
+      <c r="F10" s="8">
+        <v>45709</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
         <v>13</v>
@@ -1090,8 +1110,13 @@
       <c r="D11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>45705</v>
+      </c>
+      <c r="F11" s="8">
+        <v>45711</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7" t="s">
         <v>13</v>
@@ -1113,8 +1138,13 @@
       <c r="D12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>45705</v>
+      </c>
+      <c r="F12" s="8">
+        <v>45711</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7" t="s">
         <v>13</v>
@@ -1135,9 +1165,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -1203,14 +1231,23 @@
         <v>3.1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="8">
+        <f>E16</f>
+        <v>45719</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1218,14 +1255,27 @@
     </row>
     <row r="18" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
+      <c r="B18" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="8">
+        <f>E16</f>
+        <v>45719</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1233,14 +1283,27 @@
     </row>
     <row r="19" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="B19" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="8">
+        <f>E16</f>
+        <v>45719</v>
+      </c>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>

</xml_diff>